<commit_message>
latest changes wirh bug in combined protocol
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,40 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="0"/>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -49,35 +50,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -365,206 +357,50 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1">
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B1" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="C1" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="D1" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="E1" s="1">
-        <v>1</v>
-      </c>
-      <c r="F1" s="1">
-        <v>1.5</v>
-      </c>
-      <c r="G1" s="1">
-        <v>2</v>
-      </c>
-      <c r="H1" s="1">
-        <v>3</v>
-      </c>
-      <c r="I1" s="1">
-        <v>5</v>
-      </c>
-      <c r="J1" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2">
-        <v>2160.531007506394</v>
-      </c>
-      <c r="B2">
-        <v>2166.767114289884</v>
-      </c>
-      <c r="C2">
-        <v>2174.142424095451</v>
-      </c>
-      <c r="D2">
-        <v>2188.673780192065</v>
-      </c>
-      <c r="E2">
-        <v>2243.482516941946</v>
-      </c>
-      <c r="F2">
-        <v>2229.732558139535</v>
-      </c>
-      <c r="G2">
-        <v>2382.119897644106</v>
-      </c>
-      <c r="H2">
-        <v>2645.786668590537</v>
-      </c>
-      <c r="I2">
-        <v>5463.663003663003</v>
-      </c>
-      <c r="J2">
-        <v>102317.6711730816</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3">
-        <v>10.57896547861018</v>
-      </c>
-      <c r="B3">
-        <v>10.09630003040632</v>
-      </c>
-      <c r="C3">
-        <v>10.05989725040812</v>
-      </c>
-      <c r="D3">
-        <v>10.31679135827165</v>
-      </c>
-      <c r="E3">
-        <v>10.38278273952431</v>
-      </c>
-      <c r="F3">
-        <v>10.64824462423675</v>
-      </c>
-      <c r="G3">
-        <v>11.3245284830638</v>
-      </c>
-      <c r="H3">
-        <v>14.77335190120611</v>
-      </c>
-      <c r="I3">
-        <v>60.35278584631634</v>
-      </c>
-      <c r="J3">
-        <v>811.3132662206716</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4">
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="n">
+        <v>2055.453877484672</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="n">
+        <v>13.28862909032723</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="n">
         <v>100</v>
       </c>
-      <c r="B4">
-        <v>100</v>
-      </c>
-      <c r="C4">
-        <v>100</v>
-      </c>
-      <c r="D4">
-        <v>100</v>
-      </c>
-      <c r="E4">
-        <v>100</v>
-      </c>
-      <c r="F4">
-        <v>100</v>
-      </c>
-      <c r="G4">
-        <v>100</v>
-      </c>
-      <c r="H4">
-        <v>100</v>
-      </c>
-      <c r="I4">
-        <v>100</v>
-      </c>
-      <c r="J4">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5">
-        <v>0.6402239104358257</v>
-      </c>
-      <c r="B5">
-        <v>0.6341463414634146</v>
-      </c>
-      <c r="C5">
-        <v>0.6341463414634146</v>
-      </c>
-      <c r="D5">
-        <v>0.6341463414634146</v>
-      </c>
-      <c r="E5">
-        <v>0.6301479408236705</v>
-      </c>
-      <c r="F5">
-        <v>0.6361455417832866</v>
-      </c>
-      <c r="G5">
-        <v>0.6310275889644142</v>
-      </c>
-      <c r="H5">
-        <v>0.6421431427429029</v>
-      </c>
-      <c r="I5">
-        <v>0.6381447421031587</v>
-      </c>
-      <c r="J5">
-        <v>0.6141543382646941</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6">
-        <v>0.001281029948078255</v>
-      </c>
-      <c r="B6">
-        <v>0.001266172752443192</v>
-      </c>
-      <c r="C6">
-        <v>0.001268573395174619</v>
-      </c>
-      <c r="D6">
-        <v>0.001268050722028881</v>
-      </c>
-      <c r="E6">
-        <v>0.001260827102579292</v>
-      </c>
-      <c r="F6">
-        <v>0.001273020794011582</v>
-      </c>
-      <c r="G6">
-        <v>0.001261604761256318</v>
-      </c>
-      <c r="H6">
-        <v>0.001288753211814645</v>
-      </c>
-      <c r="I6">
-        <v>0.001282320960486716</v>
-      </c>
-      <c r="J6">
-        <v>0.001277749039477582</v>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="n">
+        <v>0.656034396560344</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="n">
+        <v>0.001311941974337574</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
need to update wait_majority
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,40 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="0"/>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -49,35 +50,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -365,206 +357,50 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1">
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B1" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="C1" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="D1" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="E1" s="1">
-        <v>1</v>
-      </c>
-      <c r="F1" s="1">
-        <v>1.5</v>
-      </c>
-      <c r="G1" s="1">
-        <v>2</v>
-      </c>
-      <c r="H1" s="1">
-        <v>3</v>
-      </c>
-      <c r="I1" s="1">
-        <v>5</v>
-      </c>
-      <c r="J1" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2">
-        <v>2160.531007506394</v>
-      </c>
-      <c r="B2">
-        <v>2166.767114289884</v>
-      </c>
-      <c r="C2">
-        <v>2174.142424095451</v>
-      </c>
-      <c r="D2">
-        <v>2188.673780192065</v>
-      </c>
-      <c r="E2">
-        <v>2243.482516941946</v>
-      </c>
-      <c r="F2">
-        <v>2229.732558139535</v>
-      </c>
-      <c r="G2">
-        <v>2382.119897644106</v>
-      </c>
-      <c r="H2">
-        <v>2645.786668590537</v>
-      </c>
-      <c r="I2">
-        <v>5463.663003663003</v>
-      </c>
-      <c r="J2">
-        <v>102317.6711730816</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3">
-        <v>10.57896547861018</v>
-      </c>
-      <c r="B3">
-        <v>10.09630003040632</v>
-      </c>
-      <c r="C3">
-        <v>10.05989725040812</v>
-      </c>
-      <c r="D3">
-        <v>10.31679135827165</v>
-      </c>
-      <c r="E3">
-        <v>10.38278273952431</v>
-      </c>
-      <c r="F3">
-        <v>10.64824462423675</v>
-      </c>
-      <c r="G3">
-        <v>11.3245284830638</v>
-      </c>
-      <c r="H3">
-        <v>14.77335190120611</v>
-      </c>
-      <c r="I3">
-        <v>60.35278584631634</v>
-      </c>
-      <c r="J3">
-        <v>811.3132662206716</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4">
-        <v>100</v>
-      </c>
-      <c r="B4">
-        <v>100</v>
-      </c>
-      <c r="C4">
-        <v>100</v>
-      </c>
-      <c r="D4">
-        <v>100</v>
-      </c>
-      <c r="E4">
-        <v>100</v>
-      </c>
-      <c r="F4">
-        <v>100</v>
-      </c>
-      <c r="G4">
-        <v>100</v>
-      </c>
-      <c r="H4">
-        <v>100</v>
-      </c>
-      <c r="I4">
-        <v>100</v>
-      </c>
-      <c r="J4">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5">
-        <v>0.6402239104358257</v>
-      </c>
-      <c r="B5">
-        <v>0.6341463414634146</v>
-      </c>
-      <c r="C5">
-        <v>0.6341463414634146</v>
-      </c>
-      <c r="D5">
-        <v>0.6341463414634146</v>
-      </c>
-      <c r="E5">
-        <v>0.6301479408236705</v>
-      </c>
-      <c r="F5">
-        <v>0.6361455417832866</v>
-      </c>
-      <c r="G5">
-        <v>0.6310275889644142</v>
-      </c>
-      <c r="H5">
-        <v>0.6421431427429029</v>
-      </c>
-      <c r="I5">
-        <v>0.6381447421031587</v>
-      </c>
-      <c r="J5">
-        <v>0.6141543382646941</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6">
-        <v>0.001281029948078255</v>
-      </c>
-      <c r="B6">
-        <v>0.001266172752443192</v>
-      </c>
-      <c r="C6">
-        <v>0.001268573395174619</v>
-      </c>
-      <c r="D6">
-        <v>0.001268050722028881</v>
-      </c>
-      <c r="E6">
-        <v>0.001260827102579292</v>
-      </c>
-      <c r="F6">
-        <v>0.001273020794011582</v>
-      </c>
-      <c r="G6">
-        <v>0.001261604761256318</v>
-      </c>
-      <c r="H6">
-        <v>0.001288753211814645</v>
-      </c>
-      <c r="I6">
-        <v>0.001282320960486716</v>
-      </c>
-      <c r="J6">
-        <v>0.001277749039477582</v>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="n">
+        <v>6790.562410329985</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="n">
+        <v>19.58875931324911</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="n">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="n">
+        <v>0.4047619047619048</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="n">
+        <v>0.0007358351729212656</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added delay histogram support
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -362,7 +362,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -370,34 +370,106 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
+      <c r="B1" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="n">
-        <v>2055.453877484672</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
+        <v>6275.982952620485</v>
+      </c>
+      <c r="B2" t="n">
+        <v>6301.83023095386</v>
+      </c>
+      <c r="C2" t="n">
+        <v>6363.372900488996</v>
+      </c>
+      <c r="D2" t="n">
+        <v>6530.920692923298</v>
+      </c>
+      <c r="E2" t="n">
+        <v>7243.782941570591</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="n">
-        <v>13.28862909032723</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
+        <v>11.41064167862783</v>
+      </c>
+      <c r="B3" t="n">
+        <v>11.4924972835958</v>
+      </c>
+      <c r="C3" t="n">
+        <v>11.84261183891548</v>
+      </c>
+      <c r="D3" t="n">
+        <v>11.64127917862189</v>
+      </c>
+      <c r="E3" t="n">
+        <v>12.266748390855</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
+        <v>250</v>
+      </c>
+      <c r="B4" t="n">
+        <v>250</v>
+      </c>
+      <c r="C4" t="n">
+        <v>250</v>
+      </c>
+      <c r="D4" t="n">
+        <v>250</v>
+      </c>
+      <c r="E4" t="n">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="n">
-        <v>0.656034396560344</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
+        <v>0.3936485081193504</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.3917046636269098</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.3932485401167907</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.3872490200783937</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.3768498520118391</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="n">
-        <v>0.001311941974337574</v>
+        <v>0.0007870296236989592</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0.0007833554177148746</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.0007864257947660684</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.0007739510642027224</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.0007532670255558446</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Plot delay vs BPT
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,41 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="0"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -50,26 +49,35 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -357,104 +365,44 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="n">
+    <row r="1" spans="1:1">
+      <c r="A1" s="1">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="C1" s="1" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="D1" s="1" t="n">
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2">
+        <v>7226.425080128205</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3">
+        <v>7.99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="n">
-        <v>21930.08368965848</v>
-      </c>
-      <c r="B2" t="n">
-        <v>25834.99544791117</v>
-      </c>
-      <c r="C2" t="n">
-        <v>22709.03891327412</v>
-      </c>
-      <c r="D2" t="n">
-        <v>27833.21037426342</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="n">
-        <v>222.7529461683799</v>
-      </c>
-      <c r="B3" t="n">
-        <v>84.061278081117</v>
-      </c>
-      <c r="C3" t="n">
-        <v>69.71747500540316</v>
-      </c>
-      <c r="D3" t="n">
-        <v>217.1202071626403</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="n">
-        <v>250</v>
-      </c>
-      <c r="B4" t="n">
-        <v>250</v>
-      </c>
-      <c r="C4" t="n">
-        <v>250</v>
-      </c>
-      <c r="D4" t="n">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="n">
-        <v>0.3950499800079968</v>
-      </c>
-      <c r="B5" t="n">
-        <v>0.3946421431427429</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0.3919392243102759</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.38984406237505</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="n">
-        <v>0.003951720464296185</v>
-      </c>
-      <c r="B6" t="n">
-        <v>0.003973125018976443</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0.003923594045467041</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.003903169049689566</v>
+    <row r="6" spans="1:1">
+      <c r="A6">
+        <v>0.0001996662892080171</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new proposal protocol option based on candidate-lottery
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -389,36 +389,36 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="n">
-        <v>6275.982952620485</v>
+        <v>1177.654280618312</v>
       </c>
       <c r="B2" t="n">
-        <v>6301.83023095386</v>
+        <v>1182.785671819263</v>
       </c>
       <c r="C2" t="n">
-        <v>6363.372900488996</v>
+        <v>1160.771254458977</v>
       </c>
       <c r="D2" t="n">
-        <v>6530.920692923298</v>
+        <v>1262.987068965517</v>
       </c>
       <c r="E2" t="n">
-        <v>7243.782941570591</v>
+        <v>1776.650564803805</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="n">
-        <v>11.41064167862783</v>
+        <v>11.09120415449529</v>
       </c>
       <c r="B3" t="n">
-        <v>11.4924972835958</v>
+        <v>11.64729817708333</v>
       </c>
       <c r="C3" t="n">
-        <v>11.84261183891548</v>
+        <v>10.89588417114039</v>
       </c>
       <c r="D3" t="n">
-        <v>11.64127917862189</v>
+        <v>12.2727420402859</v>
       </c>
       <c r="E3" t="n">
-        <v>12.266748390855</v>
+        <v>19.08367447191747</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -440,36 +440,36 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="n">
-        <v>0.3936485081193504</v>
+        <v>0.9206349206349206</v>
       </c>
       <c r="B5" t="n">
-        <v>0.3917046636269098</v>
+        <v>0.9206349206349206</v>
       </c>
       <c r="C5" t="n">
-        <v>0.3932485401167907</v>
+        <v>0.9206349206349206</v>
       </c>
       <c r="D5" t="n">
-        <v>0.3872490200783937</v>
+        <v>0.9206349206349206</v>
       </c>
       <c r="E5" t="n">
-        <v>0.3768498520118391</v>
+        <v>0.9206349206349206</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="n">
-        <v>0.0007870296236989592</v>
+        <v>0.001868703282417939</v>
       </c>
       <c r="B6" t="n">
-        <v>0.0007833554177148746</v>
+        <v>0.001860991989643175</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0007864257947660684</v>
+        <v>0.001853194746595762</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0007739510642027224</v>
+        <v>0.001859637774902975</v>
       </c>
       <c r="E6" t="n">
-        <v>0.0007532670255558446</v>
+        <v>0.00185648559205747</v>
       </c>
     </row>
   </sheetData>

</xml_diff>